<commit_message>
Add Vin.MIN=5.5V to schematic DC-DC note
</commit_message>
<xml_diff>
--- a/work/RadioSens Working Hours (STAGE 2).xlsx
+++ b/work/RadioSens Working Hours (STAGE 2).xlsx
@@ -77,7 +77,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,12 +94,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -123,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -137,10 +131,10 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -151,17 +145,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -172,6 +163,9 @@
     <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
@@ -179,9 +173,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -192,7 +183,7 @@
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -517,10 +508,10 @@
       <c r="B7" s="3">
         <v>44856.0</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="4">
         <v>0.39444444444444443</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="4">
         <v>0.44027777777777777</v>
       </c>
       <c r="E7" s="5">
@@ -529,14 +520,14 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10">
         <v>44856.0</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="4">
         <v>0.6673611111111111</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="4">
         <v>0.8833333333333333</v>
       </c>
       <c r="E8" s="5">
@@ -546,13 +537,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>44857.0</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>0.3263888888888889</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="4">
         <v>0.5458333333333333</v>
       </c>
       <c r="E9" s="5">
@@ -565,10 +556,10 @@
       <c r="B10" s="3">
         <v>44857.0</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="4">
         <v>0.7604166666666666</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="4">
         <v>0.8875</v>
       </c>
       <c r="E10" s="5">
@@ -581,10 +572,10 @@
       <c r="B11" s="3">
         <v>44858.0</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="4">
         <v>0.7631944444444444</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="4">
         <v>0.8347222222222223</v>
       </c>
       <c r="E11" s="5">
@@ -597,10 +588,10 @@
       <c r="B12" s="3">
         <v>44858.0</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="4">
         <v>0.8583333333333333</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="4">
         <v>0.9659722222222222</v>
       </c>
       <c r="E12" s="5">
@@ -613,10 +604,10 @@
       <c r="B13" s="3">
         <v>44860.0</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="4">
         <v>0.8340277777777778</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <v>0.9131944444444444</v>
       </c>
       <c r="E13" s="5">
@@ -626,1534 +617,1534 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="14"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="5"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="5"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="5"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="5"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="14"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="14"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="14"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="14"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="14"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="5"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="24"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="D34" s="10"/>
-      <c r="E34" s="25"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="24"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="D35" s="10"/>
-      <c r="E35" s="25"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="24"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="D36" s="10"/>
-      <c r="E36" s="25"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="24"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="24"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="25"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="24"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="25"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="24"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="25"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="24"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="25"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="24"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="24"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="25"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="24"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="25"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="24"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="25"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="24"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="25"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="24"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="25"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="24"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="25"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="24"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="25"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="24"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="25"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="24"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="25"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="24"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="25"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="24"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="25"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="24"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="25"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="24"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="25"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="24"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="10"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="25"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="24"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="25"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="24"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="25"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="24"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="25"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="24"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="25"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="24"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="25"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="24"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="25"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="24"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="25"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="24"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="25"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="24"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="25"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="24"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="25"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="24"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="10"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="25"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="24"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="25"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="24"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="25"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="24"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="25"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="24"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="25"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="24"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="25"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="24"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="25"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="24"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="25"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="24"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="25"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="24"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="25"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="24"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="25"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="24"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="25"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="24"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="25"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="24"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="10"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="25"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="24"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="25"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="24"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="25"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="24"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="25"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="24"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="10"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="25"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="24"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="25"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="24"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="25"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="24"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="25"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="24"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="10"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="25"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="24"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="10"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="25"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="24"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="10"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="25"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="24"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="10"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="25"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="24"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="10"/>
-      <c r="B101" s="10"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="25"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="24"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="10"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="25"/>
+      <c r="A102" s="9"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="24"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="10"/>
-      <c r="B103" s="10"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="25"/>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="24"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="10"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="25"/>
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="24"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="10"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="25"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="24"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="25"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="24"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="10"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="25"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="24"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="25"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="24"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="25"/>
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="24"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="10"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="25"/>
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="24"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="25"/>
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="24"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="25"/>
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="24"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="25"/>
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="24"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="25"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="24"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="10"/>
-      <c r="B115" s="10"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="25"/>
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="24"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="10"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-      <c r="E116" s="25"/>
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="24"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="10"/>
-      <c r="B117" s="10"/>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="25"/>
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="24"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="10"/>
-      <c r="B118" s="10"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="25"/>
+      <c r="A118" s="9"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="24"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="10"/>
-      <c r="B119" s="10"/>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="25"/>
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="24"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="10"/>
-      <c r="B120" s="10"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="25"/>
+      <c r="A120" s="9"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="24"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="10"/>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="25"/>
+      <c r="A121" s="9"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="24"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="10"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="25"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="9"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="24"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="10"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="25"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="24"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="25"/>
+      <c r="A124" s="9"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="24"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="10"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="25"/>
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="24"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="10"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="25"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="24"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="10"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="25"/>
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="24"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-      <c r="E128" s="25"/>
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="24"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="10"/>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="25"/>
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="24"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="10"/>
-      <c r="B130" s="10"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="25"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="24"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="10"/>
-      <c r="B131" s="10"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="25"/>
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="24"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="10"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="25"/>
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="24"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="10"/>
-      <c r="B133" s="10"/>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-      <c r="E133" s="25"/>
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="24"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="10"/>
-      <c r="B134" s="10"/>
-      <c r="C134" s="10"/>
-      <c r="D134" s="10"/>
-      <c r="E134" s="25"/>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="24"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="10"/>
-      <c r="B135" s="10"/>
-      <c r="C135" s="10"/>
-      <c r="D135" s="10"/>
-      <c r="E135" s="25"/>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="24"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="10"/>
-      <c r="B136" s="10"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="25"/>
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="24"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="10"/>
-      <c r="B137" s="10"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="25"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="24"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="10"/>
-      <c r="B138" s="10"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="25"/>
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="24"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="10"/>
-      <c r="B139" s="10"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
-      <c r="E139" s="25"/>
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="24"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="10"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-      <c r="E140" s="25"/>
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="24"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="10"/>
-      <c r="B141" s="10"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="10"/>
-      <c r="E141" s="25"/>
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="24"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="10"/>
-      <c r="B142" s="10"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
-      <c r="E142" s="25"/>
+      <c r="A142" s="9"/>
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="24"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="10"/>
-      <c r="B143" s="10"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-      <c r="E143" s="25"/>
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="24"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="10"/>
-      <c r="B144" s="10"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="25"/>
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="24"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="10"/>
-      <c r="B145" s="10"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="25"/>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="24"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="10"/>
-      <c r="B146" s="10"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
-      <c r="E146" s="25"/>
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="24"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="10"/>
-      <c r="B147" s="10"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-      <c r="E147" s="25"/>
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="24"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="10"/>
-      <c r="B148" s="10"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-      <c r="E148" s="25"/>
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="24"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="10"/>
-      <c r="B149" s="10"/>
-      <c r="C149" s="10"/>
-      <c r="D149" s="10"/>
-      <c r="E149" s="25"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="24"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="10"/>
-      <c r="B150" s="10"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="25"/>
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="24"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="10"/>
-      <c r="B151" s="10"/>
-      <c r="C151" s="10"/>
-      <c r="D151" s="10"/>
-      <c r="E151" s="25"/>
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="24"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="10"/>
-      <c r="B152" s="10"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-      <c r="E152" s="25"/>
+      <c r="A152" s="9"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="24"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="10"/>
-      <c r="B153" s="10"/>
-      <c r="C153" s="10"/>
-      <c r="D153" s="10"/>
-      <c r="E153" s="25"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="24"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="10"/>
-      <c r="B154" s="10"/>
-      <c r="C154" s="10"/>
-      <c r="D154" s="10"/>
-      <c r="E154" s="25"/>
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="24"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="10"/>
-      <c r="B155" s="10"/>
-      <c r="C155" s="10"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="25"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="24"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="10"/>
-      <c r="B156" s="10"/>
-      <c r="C156" s="10"/>
-      <c r="D156" s="10"/>
-      <c r="E156" s="25"/>
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="24"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="10"/>
-      <c r="B157" s="10"/>
-      <c r="C157" s="10"/>
-      <c r="D157" s="10"/>
-      <c r="E157" s="25"/>
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="24"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="10"/>
-      <c r="B158" s="10"/>
-      <c r="C158" s="10"/>
-      <c r="D158" s="10"/>
-      <c r="E158" s="25"/>
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="24"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="10"/>
-      <c r="B159" s="10"/>
-      <c r="C159" s="10"/>
-      <c r="D159" s="10"/>
-      <c r="E159" s="25"/>
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="24"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="10"/>
-      <c r="B160" s="10"/>
-      <c r="C160" s="10"/>
-      <c r="D160" s="10"/>
-      <c r="E160" s="25"/>
+      <c r="A160" s="9"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="24"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="10"/>
-      <c r="B161" s="10"/>
-      <c r="C161" s="10"/>
-      <c r="D161" s="10"/>
-      <c r="E161" s="25"/>
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="24"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="10"/>
-      <c r="B162" s="10"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-      <c r="E162" s="25"/>
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="24"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="10"/>
-      <c r="B163" s="10"/>
-      <c r="C163" s="10"/>
-      <c r="D163" s="10"/>
-      <c r="E163" s="25"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="24"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="10"/>
-      <c r="B164" s="10"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="25"/>
+      <c r="A164" s="9"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="24"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="10"/>
-      <c r="B165" s="10"/>
-      <c r="C165" s="10"/>
-      <c r="D165" s="10"/>
-      <c r="E165" s="25"/>
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="24"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="10"/>
-      <c r="B166" s="10"/>
-      <c r="C166" s="10"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="25"/>
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+      <c r="E166" s="24"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="10"/>
-      <c r="B167" s="10"/>
-      <c r="C167" s="10"/>
-      <c r="D167" s="10"/>
-      <c r="E167" s="25"/>
+      <c r="A167" s="9"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="24"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="10"/>
-      <c r="B168" s="10"/>
-      <c r="C168" s="10"/>
-      <c r="D168" s="10"/>
-      <c r="E168" s="25"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="24"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="10"/>
-      <c r="B169" s="10"/>
-      <c r="C169" s="10"/>
-      <c r="D169" s="10"/>
-      <c r="E169" s="25"/>
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="24"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="10"/>
-      <c r="B170" s="10"/>
-      <c r="C170" s="10"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="25"/>
+      <c r="A170" s="9"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="24"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="10"/>
-      <c r="B171" s="10"/>
-      <c r="C171" s="10"/>
-      <c r="D171" s="10"/>
-      <c r="E171" s="25"/>
+      <c r="A171" s="9"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="24"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="10"/>
-      <c r="B172" s="10"/>
-      <c r="C172" s="10"/>
-      <c r="D172" s="10"/>
-      <c r="E172" s="25"/>
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="24"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="10"/>
-      <c r="B173" s="10"/>
-      <c r="C173" s="10"/>
-      <c r="D173" s="10"/>
-      <c r="E173" s="25"/>
+      <c r="A173" s="9"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="24"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="10"/>
-      <c r="B174" s="10"/>
-      <c r="C174" s="10"/>
-      <c r="D174" s="10"/>
-      <c r="E174" s="25"/>
+      <c r="A174" s="9"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="24"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="10"/>
-      <c r="B175" s="10"/>
-      <c r="C175" s="10"/>
-      <c r="D175" s="10"/>
-      <c r="E175" s="25"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="24"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="10"/>
-      <c r="B176" s="10"/>
-      <c r="C176" s="10"/>
-      <c r="D176" s="10"/>
-      <c r="E176" s="25"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="24"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="10"/>
-      <c r="B177" s="10"/>
-      <c r="C177" s="10"/>
-      <c r="D177" s="10"/>
-      <c r="E177" s="25"/>
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="24"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="10"/>
-      <c r="B178" s="10"/>
-      <c r="C178" s="10"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="25"/>
+      <c r="A178" s="9"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="E178" s="24"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="10"/>
-      <c r="B179" s="10"/>
-      <c r="C179" s="10"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="25"/>
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="24"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="10"/>
-      <c r="B180" s="10"/>
-      <c r="C180" s="10"/>
-      <c r="D180" s="10"/>
-      <c r="E180" s="25"/>
+      <c r="A180" s="9"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="24"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="10"/>
-      <c r="B181" s="10"/>
-      <c r="C181" s="10"/>
-      <c r="D181" s="10"/>
-      <c r="E181" s="25"/>
+      <c r="A181" s="9"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="24"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="10"/>
-      <c r="B182" s="10"/>
-      <c r="C182" s="10"/>
-      <c r="D182" s="10"/>
-      <c r="E182" s="25"/>
+      <c r="A182" s="9"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="9"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="24"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="10"/>
-      <c r="B183" s="10"/>
-      <c r="C183" s="10"/>
-      <c r="D183" s="10"/>
-      <c r="E183" s="25"/>
+      <c r="A183" s="9"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="9"/>
+      <c r="E183" s="24"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="10"/>
-      <c r="B184" s="10"/>
-      <c r="C184" s="10"/>
-      <c r="D184" s="10"/>
-      <c r="E184" s="25"/>
+      <c r="A184" s="9"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="24"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="10"/>
-      <c r="B185" s="10"/>
-      <c r="C185" s="10"/>
-      <c r="D185" s="10"/>
-      <c r="E185" s="25"/>
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="9"/>
+      <c r="E185" s="24"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="10"/>
-      <c r="B186" s="10"/>
-      <c r="C186" s="10"/>
-      <c r="D186" s="10"/>
-      <c r="E186" s="25"/>
+      <c r="A186" s="9"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="24"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="10"/>
-      <c r="B187" s="10"/>
-      <c r="C187" s="10"/>
-      <c r="D187" s="10"/>
-      <c r="E187" s="25"/>
+      <c r="A187" s="9"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="9"/>
+      <c r="E187" s="24"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="10"/>
-      <c r="B188" s="10"/>
-      <c r="C188" s="10"/>
-      <c r="D188" s="10"/>
-      <c r="E188" s="25"/>
+      <c r="A188" s="9"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="9"/>
+      <c r="E188" s="24"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="10"/>
-      <c r="B189" s="10"/>
-      <c r="C189" s="10"/>
-      <c r="D189" s="10"/>
-      <c r="E189" s="25"/>
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="24"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="10"/>
-      <c r="B190" s="10"/>
-      <c r="C190" s="10"/>
-      <c r="D190" s="10"/>
-      <c r="E190" s="25"/>
+      <c r="A190" s="9"/>
+      <c r="B190" s="9"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="9"/>
+      <c r="E190" s="24"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="10"/>
-      <c r="B191" s="10"/>
-      <c r="C191" s="10"/>
-      <c r="D191" s="10"/>
-      <c r="E191" s="25"/>
+      <c r="A191" s="9"/>
+      <c r="B191" s="9"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
+      <c r="E191" s="24"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="10"/>
-      <c r="B192" s="10"/>
-      <c r="C192" s="10"/>
-      <c r="D192" s="10"/>
-      <c r="E192" s="25"/>
+      <c r="A192" s="9"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="9"/>
+      <c r="E192" s="24"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="10"/>
-      <c r="B193" s="10"/>
-      <c r="C193" s="10"/>
-      <c r="D193" s="10"/>
-      <c r="E193" s="25"/>
+      <c r="A193" s="9"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9"/>
+      <c r="E193" s="24"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="10"/>
-      <c r="B194" s="10"/>
-      <c r="C194" s="10"/>
-      <c r="D194" s="10"/>
-      <c r="E194" s="25"/>
+      <c r="A194" s="9"/>
+      <c r="B194" s="9"/>
+      <c r="C194" s="9"/>
+      <c r="D194" s="9"/>
+      <c r="E194" s="24"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="10"/>
-      <c r="B195" s="10"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="10"/>
-      <c r="E195" s="25"/>
+      <c r="A195" s="9"/>
+      <c r="B195" s="9"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="24"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="10"/>
-      <c r="B196" s="10"/>
-      <c r="C196" s="10"/>
-      <c r="D196" s="10"/>
-      <c r="E196" s="25"/>
+      <c r="A196" s="9"/>
+      <c r="B196" s="9"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="24"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="10"/>
-      <c r="B197" s="10"/>
-      <c r="C197" s="10"/>
-      <c r="D197" s="10"/>
-      <c r="E197" s="25"/>
+      <c r="A197" s="9"/>
+      <c r="B197" s="9"/>
+      <c r="C197" s="9"/>
+      <c r="D197" s="9"/>
+      <c r="E197" s="24"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="10"/>
-      <c r="B198" s="10"/>
-      <c r="C198" s="10"/>
-      <c r="D198" s="10"/>
-      <c r="E198" s="25"/>
+      <c r="A198" s="9"/>
+      <c r="B198" s="9"/>
+      <c r="C198" s="9"/>
+      <c r="D198" s="9"/>
+      <c r="E198" s="24"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="10"/>
-      <c r="B199" s="10"/>
-      <c r="C199" s="10"/>
-      <c r="D199" s="10"/>
-      <c r="E199" s="25"/>
+      <c r="A199" s="9"/>
+      <c r="B199" s="9"/>
+      <c r="C199" s="9"/>
+      <c r="D199" s="9"/>
+      <c r="E199" s="24"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="10"/>
-      <c r="B200" s="10"/>
-      <c r="C200" s="10"/>
-      <c r="D200" s="10"/>
-      <c r="E200" s="25"/>
+      <c r="A200" s="9"/>
+      <c r="B200" s="9"/>
+      <c r="C200" s="9"/>
+      <c r="D200" s="9"/>
+      <c r="E200" s="24"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="10"/>
-      <c r="B201" s="10"/>
-      <c r="C201" s="10"/>
-      <c r="D201" s="10"/>
-      <c r="E201" s="25"/>
+      <c r="A201" s="9"/>
+      <c r="B201" s="9"/>
+      <c r="C201" s="9"/>
+      <c r="D201" s="9"/>
+      <c r="E201" s="24"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="10"/>
-      <c r="B202" s="10"/>
-      <c r="C202" s="10"/>
-      <c r="D202" s="10"/>
-      <c r="E202" s="25"/>
+      <c r="A202" s="9"/>
+      <c r="B202" s="9"/>
+      <c r="C202" s="9"/>
+      <c r="D202" s="9"/>
+      <c r="E202" s="24"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="10"/>
-      <c r="B203" s="10"/>
-      <c r="C203" s="10"/>
-      <c r="D203" s="10"/>
-      <c r="E203" s="25"/>
+      <c r="A203" s="9"/>
+      <c r="B203" s="9"/>
+      <c r="C203" s="9"/>
+      <c r="D203" s="9"/>
+      <c r="E203" s="24"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="10"/>
-      <c r="B204" s="10"/>
-      <c r="C204" s="10"/>
-      <c r="D204" s="10"/>
-      <c r="E204" s="25"/>
+      <c r="A204" s="9"/>
+      <c r="B204" s="9"/>
+      <c r="C204" s="9"/>
+      <c r="D204" s="9"/>
+      <c r="E204" s="24"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="10"/>
-      <c r="B205" s="10"/>
-      <c r="C205" s="10"/>
-      <c r="D205" s="10"/>
-      <c r="E205" s="25"/>
+      <c r="A205" s="9"/>
+      <c r="B205" s="9"/>
+      <c r="C205" s="9"/>
+      <c r="D205" s="9"/>
+      <c r="E205" s="24"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="10"/>
-      <c r="B206" s="10"/>
-      <c r="C206" s="10"/>
-      <c r="D206" s="10"/>
-      <c r="E206" s="25"/>
+      <c r="A206" s="9"/>
+      <c r="B206" s="9"/>
+      <c r="C206" s="9"/>
+      <c r="D206" s="9"/>
+      <c r="E206" s="24"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="10"/>
-      <c r="B207" s="10"/>
-      <c r="C207" s="10"/>
-      <c r="D207" s="10"/>
-      <c r="E207" s="25"/>
+      <c r="A207" s="9"/>
+      <c r="B207" s="9"/>
+      <c r="C207" s="9"/>
+      <c r="D207" s="9"/>
+      <c r="E207" s="24"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="10"/>
-      <c r="B208" s="10"/>
-      <c r="C208" s="10"/>
-      <c r="D208" s="10"/>
-      <c r="E208" s="25"/>
+      <c r="A208" s="9"/>
+      <c r="B208" s="9"/>
+      <c r="C208" s="9"/>
+      <c r="D208" s="9"/>
+      <c r="E208" s="24"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="10"/>
-      <c r="B209" s="10"/>
-      <c r="C209" s="10"/>
-      <c r="D209" s="10"/>
-      <c r="E209" s="25"/>
+      <c r="A209" s="9"/>
+      <c r="B209" s="9"/>
+      <c r="C209" s="9"/>
+      <c r="D209" s="9"/>
+      <c r="E209" s="24"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="10"/>
-      <c r="B210" s="10"/>
-      <c r="C210" s="10"/>
-      <c r="D210" s="10"/>
-      <c r="E210" s="25"/>
+      <c r="A210" s="9"/>
+      <c r="B210" s="9"/>
+      <c r="C210" s="9"/>
+      <c r="D210" s="9"/>
+      <c r="E210" s="24"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="10"/>
-      <c r="B211" s="10"/>
-      <c r="C211" s="10"/>
-      <c r="D211" s="10"/>
-      <c r="E211" s="25"/>
+      <c r="A211" s="9"/>
+      <c r="B211" s="9"/>
+      <c r="C211" s="9"/>
+      <c r="D211" s="9"/>
+      <c r="E211" s="24"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="10"/>
-      <c r="B212" s="10"/>
-      <c r="C212" s="10"/>
-      <c r="D212" s="10"/>
-      <c r="E212" s="25"/>
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
+      <c r="C212" s="9"/>
+      <c r="D212" s="9"/>
+      <c r="E212" s="24"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="10"/>
-      <c r="B213" s="10"/>
-      <c r="C213" s="10"/>
-      <c r="D213" s="10"/>
-      <c r="E213" s="25"/>
+      <c r="A213" s="9"/>
+      <c r="B213" s="9"/>
+      <c r="C213" s="9"/>
+      <c r="D213" s="9"/>
+      <c r="E213" s="24"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="10"/>
-      <c r="B214" s="10"/>
-      <c r="C214" s="10"/>
-      <c r="D214" s="10"/>
-      <c r="E214" s="25"/>
+      <c r="A214" s="9"/>
+      <c r="B214" s="9"/>
+      <c r="C214" s="9"/>
+      <c r="D214" s="9"/>
+      <c r="E214" s="24"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="10"/>
-      <c r="B215" s="10"/>
-      <c r="C215" s="10"/>
-      <c r="D215" s="10"/>
-      <c r="E215" s="25"/>
+      <c r="A215" s="9"/>
+      <c r="B215" s="9"/>
+      <c r="C215" s="9"/>
+      <c r="D215" s="9"/>
+      <c r="E215" s="24"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="10"/>
-      <c r="B216" s="10"/>
-      <c r="C216" s="10"/>
-      <c r="D216" s="10"/>
-      <c r="E216" s="25"/>
+      <c r="A216" s="9"/>
+      <c r="B216" s="9"/>
+      <c r="C216" s="9"/>
+      <c r="D216" s="9"/>
+      <c r="E216" s="24"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="10"/>
-      <c r="B217" s="10"/>
-      <c r="C217" s="10"/>
-      <c r="D217" s="10"/>
-      <c r="E217" s="25"/>
+      <c r="A217" s="9"/>
+      <c r="B217" s="9"/>
+      <c r="C217" s="9"/>
+      <c r="D217" s="9"/>
+      <c r="E217" s="24"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="10"/>
-      <c r="B218" s="10"/>
-      <c r="C218" s="10"/>
-      <c r="D218" s="10"/>
-      <c r="E218" s="25"/>
+      <c r="A218" s="9"/>
+      <c r="B218" s="9"/>
+      <c r="C218" s="9"/>
+      <c r="D218" s="9"/>
+      <c r="E218" s="24"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="10"/>
-      <c r="B219" s="10"/>
-      <c r="C219" s="10"/>
-      <c r="D219" s="10"/>
-      <c r="E219" s="25"/>
+      <c r="A219" s="9"/>
+      <c r="B219" s="9"/>
+      <c r="C219" s="9"/>
+      <c r="D219" s="9"/>
+      <c r="E219" s="24"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="10"/>
-      <c r="B220" s="10"/>
-      <c r="C220" s="10"/>
-      <c r="D220" s="10"/>
-      <c r="E220" s="25"/>
+      <c r="A220" s="9"/>
+      <c r="B220" s="9"/>
+      <c r="C220" s="9"/>
+      <c r="D220" s="9"/>
+      <c r="E220" s="24"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="10"/>
-      <c r="B221" s="10"/>
-      <c r="C221" s="10"/>
-      <c r="D221" s="10"/>
-      <c r="E221" s="25"/>
+      <c r="A221" s="9"/>
+      <c r="B221" s="9"/>
+      <c r="C221" s="9"/>
+      <c r="D221" s="9"/>
+      <c r="E221" s="24"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="10"/>
-      <c r="B222" s="10"/>
-      <c r="C222" s="10"/>
-      <c r="D222" s="10"/>
-      <c r="E222" s="25"/>
+      <c r="A222" s="9"/>
+      <c r="B222" s="9"/>
+      <c r="C222" s="9"/>
+      <c r="D222" s="9"/>
+      <c r="E222" s="24"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="10"/>
-      <c r="B223" s="10"/>
-      <c r="C223" s="10"/>
-      <c r="D223" s="10"/>
-      <c r="E223" s="25"/>
+      <c r="A223" s="9"/>
+      <c r="B223" s="9"/>
+      <c r="C223" s="9"/>
+      <c r="D223" s="9"/>
+      <c r="E223" s="24"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="10"/>
-      <c r="B224" s="10"/>
-      <c r="C224" s="10"/>
-      <c r="D224" s="10"/>
-      <c r="E224" s="25"/>
+      <c r="A224" s="9"/>
+      <c r="B224" s="9"/>
+      <c r="C224" s="9"/>
+      <c r="D224" s="9"/>
+      <c r="E224" s="24"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="10"/>
-      <c r="B225" s="10"/>
-      <c r="C225" s="10"/>
-      <c r="D225" s="10"/>
-      <c r="E225" s="25"/>
+      <c r="A225" s="9"/>
+      <c r="B225" s="9"/>
+      <c r="C225" s="9"/>
+      <c r="D225" s="9"/>
+      <c r="E225" s="24"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="10"/>
-      <c r="B226" s="10"/>
-      <c r="C226" s="10"/>
-      <c r="D226" s="10"/>
-      <c r="E226" s="25"/>
+      <c r="A226" s="9"/>
+      <c r="B226" s="9"/>
+      <c r="C226" s="9"/>
+      <c r="D226" s="9"/>
+      <c r="E226" s="24"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="10"/>
-      <c r="B227" s="10"/>
-      <c r="C227" s="10"/>
-      <c r="D227" s="10"/>
-      <c r="E227" s="25"/>
+      <c r="A227" s="9"/>
+      <c r="B227" s="9"/>
+      <c r="C227" s="9"/>
+      <c r="D227" s="9"/>
+      <c r="E227" s="24"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="10"/>
-      <c r="B228" s="10"/>
-      <c r="C228" s="10"/>
-      <c r="D228" s="10"/>
-      <c r="E228" s="25"/>
+      <c r="A228" s="9"/>
+      <c r="B228" s="9"/>
+      <c r="C228" s="9"/>
+      <c r="D228" s="9"/>
+      <c r="E228" s="24"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="10"/>
-      <c r="B229" s="10"/>
-      <c r="C229" s="10"/>
-      <c r="D229" s="10"/>
-      <c r="E229" s="25"/>
+      <c r="A229" s="9"/>
+      <c r="B229" s="9"/>
+      <c r="C229" s="9"/>
+      <c r="D229" s="9"/>
+      <c r="E229" s="24"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="10"/>
-      <c r="B230" s="10"/>
-      <c r="C230" s="10"/>
-      <c r="D230" s="10"/>
-      <c r="E230" s="25"/>
+      <c r="A230" s="9"/>
+      <c r="B230" s="9"/>
+      <c r="C230" s="9"/>
+      <c r="D230" s="9"/>
+      <c r="E230" s="24"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="10"/>
-      <c r="B231" s="10"/>
-      <c r="C231" s="10"/>
-      <c r="D231" s="10"/>
-      <c r="E231" s="25"/>
+      <c r="A231" s="9"/>
+      <c r="B231" s="9"/>
+      <c r="C231" s="9"/>
+      <c r="D231" s="9"/>
+      <c r="E231" s="24"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="10"/>
-      <c r="B232" s="10"/>
-      <c r="C232" s="10"/>
-      <c r="D232" s="10"/>
-      <c r="E232" s="25"/>
+      <c r="A232" s="9"/>
+      <c r="B232" s="9"/>
+      <c r="C232" s="9"/>
+      <c r="D232" s="9"/>
+      <c r="E232" s="24"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="10"/>
-      <c r="B233" s="10"/>
-      <c r="C233" s="10"/>
-      <c r="D233" s="10"/>
-      <c r="E233" s="25"/>
+      <c r="A233" s="9"/>
+      <c r="B233" s="9"/>
+      <c r="C233" s="9"/>
+      <c r="D233" s="9"/>
+      <c r="E233" s="24"/>
     </row>
     <row r="234" ht="15.75" customHeight="1"/>
     <row r="235" ht="15.75" customHeight="1"/>

</xml_diff>